<commit_message>
save progress, create more charts
</commit_message>
<xml_diff>
--- a/Respostas.xlsx
+++ b/Respostas.xlsx
@@ -829,7 +829,7 @@
   </sheetPr>
   <dimension ref="A1:AD77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H64" activeCellId="0" sqref="H64"/>
     </sheetView>
   </sheetViews>
@@ -6260,10 +6260,7 @@
       <c r="E64" s="11"/>
       <c r="F64" s="11"/>
       <c r="G64" s="11"/>
-      <c r="H64" s="11" t="n">
-        <f aca="false">COUNTIF(H2:HG6463, "2")</f>
-        <v>24</v>
-      </c>
+      <c r="H64" s="11"/>
       <c r="I64" s="11"/>
       <c r="J64" s="11"/>
       <c r="K64" s="11"/>

</xml_diff>